<commit_message>
change number of search
</commit_message>
<xml_diff>
--- a/binary_search/CPE360-search.xlsx
+++ b/binary_search/CPE360-search.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>Size of array</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>sorted time (ms)</t>
+  </si>
+  <si>
+    <t>Size of search number</t>
   </si>
 </sst>
 </file>
@@ -95,7 +98,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>search time(million second) and binary search time (ms)</a:t>
+              <a:t>10000 repeat search time(million second) and binary search time (ms)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -111,7 +114,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$I$2</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -126,18 +129,18 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$H$3:$H$10</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>Sheet1!$I$3:$I$10</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="817847068"/>
-        <c:axId val="2147431741"/>
+        <c:axId val="1511619711"/>
+        <c:axId val="1272138221"/>
       </c:barChart>
       <c:lineChart>
         <c:varyColors val="0"/>
@@ -146,7 +149,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$J$2</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -161,22 +164,22 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$H$3:$H$10</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$11</c:f>
+              <c:f>Sheet1!$J$3:$J$10</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="817847068"/>
-        <c:axId val="2147431741"/>
+        <c:axId val="1511619711"/>
+        <c:axId val="1272138221"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="817847068"/>
+        <c:axId val="1511619711"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -228,10 +231,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2147431741"/>
+        <c:crossAx val="1272138221"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2147431741"/>
+        <c:axId val="1272138221"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -306,7 +309,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="817847068"/>
+        <c:crossAx val="1511619711"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -356,7 +359,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>Sorted time for the array</a:t>
+              <a:t>10000 repeat sorted time (ms) vs. Size of array</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -372,7 +375,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$K$2</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -387,21 +390,21 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$H$3:$H$10</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:f>Sheet1!$K$3:$K$10</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1664377246"/>
-        <c:axId val="67529408"/>
+        <c:axId val="808907728"/>
+        <c:axId val="889490563"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1664377246"/>
+        <c:axId val="808907728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,7 +431,7 @@
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:rPr>
-                  <a:t/>
+                  <a:t>Size of array</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -453,10 +456,265 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67529408"/>
+        <c:crossAx val="889490563"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67529408"/>
+        <c:axId val="889490563"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>sorted time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="808907728"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>search time(million second) and binary search time (ms)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$2</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$12</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$2</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$12</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="1703433712"/>
+        <c:axId val="1090313069"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1703433712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Size of array</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1090313069"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1090313069"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -531,7 +789,232 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1664377246"/>
+        <c:crossAx val="1703433712"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>sorted time (ms) vs. Size of array</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$2</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$12</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="1935161013"/>
+        <c:axId val="585384196"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1935161013"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Size of array</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="585384196"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="585384196"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>sorted time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1935161013"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -561,10 +1044,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
@@ -586,10 +1069,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>847725</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
@@ -604,6 +1087,56 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 4" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -819,39 +1352,44 @@
     <col customWidth="1" min="2" max="2" width="24.25"/>
     <col customWidth="1" min="3" max="3" width="20.25"/>
     <col customWidth="1" min="4" max="4" width="13.63"/>
+    <col customWidth="1" min="5" max="5" width="18.63"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.0</v>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="B3" s="1">
         <v>0.0</v>
@@ -860,12 +1398,30 @@
         <v>0.0</v>
       </c>
       <c r="D3" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="1">
         <v>1.0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>147.0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>156.0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>10000.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
       <c r="B4" s="1">
         <v>0.0</v>
@@ -874,105 +1430,251 @@
         <v>0.0</v>
       </c>
       <c r="D4" s="1">
-        <v>3.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>280.0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>156.0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>10000.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>100.0</v>
+        <v>10.0</v>
       </c>
       <c r="B5" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C5" s="1">
         <v>0.0</v>
       </c>
       <c r="D5" s="1">
-        <v>31.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>491.0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>309.0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>10000.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>1000.0</v>
+        <v>100.0</v>
       </c>
       <c r="B6" s="1">
-        <v>9.0</v>
+        <v>1.0</v>
       </c>
       <c r="C6" s="1">
         <v>0.0</v>
       </c>
       <c r="D6" s="1">
-        <v>381.0</v>
+        <v>31.0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2255.0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1116.0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>10000.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>10000.0</v>
+        <v>1000.0</v>
       </c>
       <c r="B7" s="1">
-        <v>83.0</v>
+        <v>9.0</v>
       </c>
       <c r="C7" s="1">
         <v>0.0</v>
       </c>
       <c r="D7" s="1">
-        <v>2085.0</v>
+        <v>381.0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1000.0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>8909.0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>206.0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>10000.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>100000.0</v>
+        <v>10000.0</v>
       </c>
       <c r="B8" s="1">
-        <v>158.0</v>
+        <v>83.0</v>
       </c>
       <c r="C8" s="1">
         <v>0.0</v>
       </c>
       <c r="D8" s="1">
-        <v>10794.0</v>
+        <v>2085.0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>10000.0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>85037.0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>492.0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>844.0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>10000.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>1000000.0</v>
+        <v>100000.0</v>
       </c>
       <c r="B9" s="1">
-        <v>3081.0</v>
+        <v>158.0</v>
       </c>
       <c r="C9" s="1">
         <v>0.0</v>
       </c>
       <c r="D9" s="1">
-        <v>136059.0</v>
+        <v>10794.0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>100000.0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1012964.0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>489.0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>10794.0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>10000.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>1.0E7</v>
+        <v>1000000.0</v>
       </c>
       <c r="B10" s="1">
-        <v>8703.0</v>
+        <v>3081.0</v>
       </c>
       <c r="C10" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>136059.0</v>
+      </c>
+      <c r="E10" s="1">
         <v>1.0</v>
       </c>
-      <c r="D10" s="1">
-        <v>1473720.0</v>
+      <c r="H10" s="1">
+        <v>1000000.0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>5511947.0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>571.0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>136059.0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>10000.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>1.0E8</v>
+        <v>1.0E7</v>
       </c>
       <c r="B11" s="1">
-        <v>64518.0</v>
+        <v>8703.0</v>
       </c>
       <c r="C11" s="1">
         <v>1.0</v>
       </c>
       <c r="D11" s="1">
+        <v>1473720.0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>1.0E8</v>
+      </c>
+      <c r="B12" s="1">
+        <v>64518.0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="1">
         <v>1.6728941E7</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>